<commit_message>
Optimization v0 - functional - YA
</commit_message>
<xml_diff>
--- a/markowitz.xlsx
+++ b/markowitz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Go\src\pusher\defi_aggregator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6796A4E-B7A5-445A-ABE8-35454378B6BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5F61C0-D399-4706-B519-FA01E2F8751D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{C4A1E074-6D0A-432D-9438-FC70F5EA2A1C}"/>
   </bookViews>
@@ -151,8 +151,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -198,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -206,18 +207,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27074708-22F9-4BF3-8C71-EE2061120A13}">
   <dimension ref="D4:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="G23" workbookViewId="0">
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -551,8 +549,9 @@
     <col min="12" max="12" width="8.76953125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.58984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.58984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.31640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="4:20" x14ac:dyDescent="0.75">
@@ -587,23 +586,23 @@
       </c>
       <c r="O5" s="2">
         <f>I17</f>
-        <v>0.29145275964966716</v>
-      </c>
-      <c r="Q5" s="5">
-        <f>COVAR($I$6:$I$9,I$6:I$9)*250</f>
-        <v>2.0728323332983741E-2</v>
-      </c>
-      <c r="R5" s="6">
-        <f t="shared" ref="R5:T5" si="0">COVAR($I$6:$I$9,J$6:J$9)*250</f>
-        <v>-0.92635057610783578</v>
-      </c>
-      <c r="S5" s="6">
-        <f t="shared" si="0"/>
-        <v>0.19611760555083257</v>
-      </c>
-      <c r="T5" s="5">
-        <f t="shared" si="0"/>
-        <v>-6.4341010889389636E-5</v>
+        <v>0.39171250896915266</v>
+      </c>
+      <c r="Q5" s="8">
+        <f>COVAR($I$7:$I$9,I$7:I$9)</f>
+        <v>1.0994700649692729E-4</v>
+      </c>
+      <c r="R5" s="8">
+        <f>COVAR($I$7:$I$9,J$7:J$9)</f>
+        <v>-5.0365905943230869E-3</v>
+      </c>
+      <c r="S5" s="8">
+        <f>COVAR($I$7:$I$9,K$7:K$9)*250</f>
+        <v>0.25818945330086351</v>
+      </c>
+      <c r="T5" s="8">
+        <f>COVAR($I$7:$I$9,L$7:L$9)*250</f>
+        <v>1.4994717043988065E-6</v>
       </c>
     </row>
     <row r="6" spans="4:20" x14ac:dyDescent="0.75">
@@ -619,40 +618,28 @@
       <c r="G6">
         <v>111.4</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
       <c r="N6" t="s">
         <v>3</v>
       </c>
       <c r="O6" s="2">
         <f>J17</f>
-        <v>46.345830665813061</v>
-      </c>
-      <c r="Q6" s="6">
-        <f>COVAR($J$6:$J$9,I$6:I$9)*250</f>
-        <v>-0.92635057610783578</v>
-      </c>
-      <c r="R6" s="5">
-        <f t="shared" ref="R6:T6" si="1">COVAR($J$6:$J$9,J$6:J$9)*250</f>
-        <v>52.255705992851134</v>
-      </c>
-      <c r="S6" s="5">
-        <f t="shared" si="1"/>
-        <v>-4.8302450730582747</v>
-      </c>
-      <c r="T6" s="5">
-        <f t="shared" si="1"/>
-        <v>-1.0450534201256923E-2</v>
+        <v>62.288796414852754</v>
+      </c>
+      <c r="Q6" s="8">
+        <f>COVAR($J$7:$J$9,I$7:I$9)</f>
+        <v>-5.0365905943230869E-3</v>
+      </c>
+      <c r="R6" s="9">
+        <f t="shared" ref="R6:T6" si="0">COVAR($J$7:$J$9,J$7:J$9)*250</f>
+        <v>65.855721732505117</v>
+      </c>
+      <c r="S6" s="9">
+        <f t="shared" si="0"/>
+        <v>-6.9651909000747221</v>
+      </c>
+      <c r="T6" s="9">
+        <f t="shared" si="0"/>
+        <v>-5.3885192059466329E-5</v>
       </c>
     </row>
     <row r="7" spans="4:20" x14ac:dyDescent="0.75">
@@ -673,15 +660,15 @@
         <v>9.009009009008917E-3</v>
       </c>
       <c r="J7" s="1">
-        <f t="shared" ref="J7:L7" si="2">E7/E6-1</f>
+        <f t="shared" ref="J7:L7" si="1">E7/E6-1</f>
         <v>0.12676056338028174</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.23548387096774182</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" si="2"/>
+        <f>G7/G6-1</f>
         <v>-8.9766606822272443E-4</v>
       </c>
       <c r="N7" t="s">
@@ -689,23 +676,23 @@
       </c>
       <c r="O7" s="2">
         <f>K17</f>
-        <v>6.3702834161542956</v>
-      </c>
-      <c r="Q7" s="6">
-        <f>COVAR($K$6:$K$9,I$6:I$9)*250</f>
-        <v>0.19611760555083257</v>
-      </c>
-      <c r="R7" s="7">
-        <f t="shared" ref="R7:T7" si="3">COVAR($K$6:$K$9,J$6:J$9)*250</f>
-        <v>-4.8302450730582747</v>
-      </c>
-      <c r="S7" s="5">
-        <f t="shared" si="3"/>
-        <v>4.0419706397230204</v>
-      </c>
-      <c r="T7" s="5">
-        <f t="shared" si="3"/>
-        <v>-1.413714467059526E-3</v>
+        <v>8.5616609113113729</v>
+      </c>
+      <c r="Q7" s="9">
+        <f>COVAR($K$7:$K$9,I$7:I$9)*250</f>
+        <v>0.25818945330086351</v>
+      </c>
+      <c r="R7" s="9">
+        <f t="shared" ref="R7:T7" si="2">COVAR($K$7:$K$9,J$7:J$9)*250</f>
+        <v>-6.9651909000747221</v>
+      </c>
+      <c r="S7" s="9">
+        <f t="shared" si="2"/>
+        <v>5.3171510559824604</v>
+      </c>
+      <c r="T7" s="9">
+        <f t="shared" si="2"/>
+        <v>2.2890097962049293E-5</v>
       </c>
     </row>
     <row r="8" spans="4:20" x14ac:dyDescent="0.75">
@@ -722,19 +709,19 @@
         <v>111.2</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" ref="I8:I9" si="4">D8/D7-1</f>
+        <f t="shared" ref="I8:I9" si="3">D8/D7-1</f>
         <v>8.9285714285716189E-3</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" ref="J8:J9" si="5">E8/E7-1</f>
+        <f t="shared" ref="J8:J9" si="4">E8/E7-1</f>
         <v>-0.3125</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" ref="K8:K9" si="6">F8/F7-1</f>
+        <f t="shared" ref="K8:K9" si="5">F8/F7-1</f>
         <v>-2.8720626631853596E-2</v>
       </c>
       <c r="L8" s="1">
-        <f t="shared" ref="L8:L9" si="7">G8/G7-1</f>
+        <f>G8/G7-1</f>
         <v>-8.9847259658570877E-4</v>
       </c>
       <c r="N8" t="s">
@@ -742,23 +729,23 @@
       </c>
       <c r="O8" s="2">
         <f>L17</f>
-        <v>-0.16846370252175669</v>
-      </c>
-      <c r="Q8" s="5">
-        <f>COVAR($L$6:$L$9,I$6:I$9)*250</f>
-        <v>-6.4341010889389636E-5</v>
-      </c>
-      <c r="R8" s="5">
-        <f t="shared" ref="R8:T8" si="8">COVAR($L$6:$L$9,J$6:J$9)*250</f>
-        <v>-1.0450534201256923E-2</v>
-      </c>
-      <c r="S8" s="5">
-        <f t="shared" si="8"/>
-        <v>-1.413714467059526E-3</v>
-      </c>
-      <c r="T8" s="5">
-        <f t="shared" si="8"/>
-        <v>3.7840106880449129E-5</v>
+        <v>-0.22641521618924099</v>
+      </c>
+      <c r="Q8" s="8">
+        <f>COVAR($L$7:$L$9,I$7:I$9)*250</f>
+        <v>1.4994717043988065E-6</v>
+      </c>
+      <c r="R8" s="8">
+        <f t="shared" ref="R8:T8" si="6">COVAR($L$7:$L$9,J$7:J$9)*250</f>
+        <v>-5.3885192059466329E-5</v>
+      </c>
+      <c r="S8" s="8">
+        <f t="shared" si="6"/>
+        <v>2.2890097962049293E-5</v>
+      </c>
+      <c r="T8" s="8">
+        <f>COVAR($L$7:$L$9,L$7:L$9)*250</f>
+        <v>1.0860977407865404E-10</v>
       </c>
     </row>
     <row r="9" spans="4:20" x14ac:dyDescent="0.75">
@@ -775,19 +762,19 @@
         <v>111.1</v>
       </c>
       <c r="I9" s="1">
+        <f t="shared" si="3"/>
+        <v>-1.3274336283185861E-2</v>
+      </c>
+      <c r="J9" s="1">
         <f t="shared" si="4"/>
-        <v>-1.3274336283185861E-2</v>
-      </c>
-      <c r="J9" s="1">
+        <v>0.92727272727272725</v>
+      </c>
+      <c r="K9" s="1">
         <f t="shared" si="5"/>
-        <v>0.92727272727272725</v>
-      </c>
-      <c r="K9" s="1">
-        <f t="shared" si="6"/>
         <v>-0.10483870967741948</v>
       </c>
       <c r="L9" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="L8:L9" si="7">G9/G8-1</f>
         <v>-8.9928057553967378E-4</v>
       </c>
     </row>
@@ -802,41 +789,41 @@
     <row r="11" spans="4:20" x14ac:dyDescent="0.75">
       <c r="I11">
         <f>_xlfn.VAR.S(I6:I9)</f>
-        <v>1.1055105777591329E-4</v>
+        <v>1.6492050974539093E-4</v>
       </c>
       <c r="J11">
-        <f t="shared" ref="J11:L11" si="9">_xlfn.VAR.S(J6:J9)</f>
-        <v>0.27869709862853936</v>
+        <f t="shared" ref="J11:L11" si="8">_xlfn.VAR.S(J6:J9)</f>
+        <v>0.39513433039503071</v>
       </c>
       <c r="K11">
-        <f t="shared" si="9"/>
-        <v>2.1557176745189435E-2</v>
+        <f t="shared" si="8"/>
+        <v>3.1902906335894765E-2</v>
       </c>
       <c r="L11">
-        <f t="shared" si="9"/>
-        <v>2.0181390336239537E-7</v>
+        <f t="shared" si="8"/>
+        <v>6.516586444719243E-13</v>
       </c>
     </row>
     <row r="12" spans="4:20" x14ac:dyDescent="0.75">
       <c r="I12">
         <f>I11*250</f>
-        <v>2.7637764443978322E-2</v>
+        <v>4.1230127436347734E-2</v>
       </c>
       <c r="J12">
-        <f t="shared" ref="J12:L12" si="10">J11*250</f>
-        <v>69.674274657134845</v>
+        <f t="shared" ref="J12:L12" si="9">J11*250</f>
+        <v>98.783582598757675</v>
       </c>
       <c r="K12">
-        <f t="shared" si="10"/>
-        <v>5.3892941862973585</v>
+        <f t="shared" si="9"/>
+        <v>7.9757265839736915</v>
       </c>
       <c r="L12">
-        <f t="shared" si="10"/>
-        <v>5.0453475840598843E-5</v>
+        <f t="shared" si="9"/>
+        <v>1.6291466111798109E-10</v>
       </c>
       <c r="O12" s="2">
         <f>_xlfn.COVARIANCE.P(I6:I9,J6:J9)</f>
-        <v>-3.705402304431343E-3</v>
+        <v>-5.0365905943230869E-3</v>
       </c>
     </row>
     <row r="14" spans="4:20" x14ac:dyDescent="0.75">
@@ -845,37 +832,37 @@
       </c>
       <c r="I14" s="2">
         <f>AVERAGE(I6:I9)</f>
-        <v>1.1658110385986686E-3</v>
+        <v>1.5544147181315582E-3</v>
       </c>
       <c r="J14" s="2">
         <f>AVERAGE(J6:J9)</f>
-        <v>0.18538332266325225</v>
+        <v>0.24717776355100299</v>
       </c>
       <c r="K14" s="2">
-        <f t="shared" ref="J14:L14" si="11">AVERAGE(K6:K9)</f>
-        <v>2.5481133664617184E-2</v>
+        <f t="shared" ref="J14:L14" si="10">AVERAGE(K6:K9)</f>
+        <v>3.3974844886156243E-2</v>
       </c>
       <c r="L14" s="2">
-        <f t="shared" si="11"/>
-        <v>-6.7385481008702675E-4</v>
+        <f t="shared" si="10"/>
+        <v>-8.9847308011603566E-4</v>
       </c>
     </row>
     <row r="15" spans="4:20" x14ac:dyDescent="0.75">
       <c r="I15" s="2">
         <f>_xlfn.VAR.S(I6:I9)</f>
-        <v>1.1055105777591329E-4</v>
+        <v>1.6492050974539093E-4</v>
       </c>
       <c r="J15" s="2">
-        <f t="shared" ref="J15:L15" si="12">_xlfn.VAR.S(J6:J9)</f>
-        <v>0.27869709862853936</v>
+        <f t="shared" ref="J15:L15" si="11">_xlfn.VAR.S(J6:J9)</f>
+        <v>0.39513433039503071</v>
       </c>
       <c r="K15" s="2">
-        <f t="shared" si="12"/>
-        <v>2.1557176745189435E-2</v>
+        <f t="shared" si="11"/>
+        <v>3.1902906335894765E-2</v>
       </c>
       <c r="L15" s="2">
-        <f t="shared" si="12"/>
-        <v>2.0181390336239537E-7</v>
+        <f t="shared" si="11"/>
+        <v>6.516586444719243E-13</v>
       </c>
     </row>
     <row r="16" spans="4:20" x14ac:dyDescent="0.75">
@@ -888,7 +875,7 @@
       </c>
       <c r="O16" s="2">
         <f>O5</f>
-        <v>0.29145275964966716</v>
+        <v>0.39171250896915266</v>
       </c>
     </row>
     <row r="17" spans="8:15" x14ac:dyDescent="0.75">
@@ -896,52 +883,52 @@
         <v>1</v>
       </c>
       <c r="I17" s="2">
-        <f>I14*250</f>
-        <v>0.29145275964966716</v>
+        <f>I14*252</f>
+        <v>0.39171250896915266</v>
       </c>
       <c r="J17" s="2">
-        <f t="shared" ref="J17:L17" si="13">J14*250</f>
-        <v>46.345830665813061</v>
+        <f t="shared" ref="J17:L17" si="12">J14*252</f>
+        <v>62.288796414852754</v>
       </c>
       <c r="K17" s="2">
-        <f t="shared" si="13"/>
-        <v>6.3702834161542956</v>
+        <f t="shared" si="12"/>
+        <v>8.5616609113113729</v>
       </c>
       <c r="L17" s="2">
-        <f t="shared" si="13"/>
-        <v>-0.16846370252175669</v>
+        <f t="shared" si="12"/>
+        <v>-0.22641521618924099</v>
       </c>
       <c r="N17">
         <v>0.25</v>
       </c>
       <c r="O17" s="2">
-        <f t="shared" ref="O17:O19" si="14">O6</f>
-        <v>46.345830665813061</v>
+        <f t="shared" ref="O17:O19" si="13">O6</f>
+        <v>62.288796414852754</v>
       </c>
     </row>
     <row r="18" spans="8:15" x14ac:dyDescent="0.75">
       <c r="I18" s="2">
         <f>I15*250</f>
-        <v>2.7637764443978322E-2</v>
+        <v>4.1230127436347734E-2</v>
       </c>
       <c r="J18" s="2">
-        <f t="shared" ref="J18:L18" si="15">J15*250</f>
-        <v>69.674274657134845</v>
+        <f t="shared" ref="J18:L18" si="14">J15*250</f>
+        <v>98.783582598757675</v>
       </c>
       <c r="K18" s="2">
-        <f t="shared" si="15"/>
-        <v>5.3892941862973585</v>
+        <f t="shared" si="14"/>
+        <v>7.9757265839736915</v>
       </c>
       <c r="L18" s="2">
-        <f t="shared" si="15"/>
-        <v>5.0453475840598843E-5</v>
+        <f t="shared" si="14"/>
+        <v>1.6291466111798109E-10</v>
       </c>
       <c r="N18">
         <v>0.25</v>
       </c>
       <c r="O18" s="2">
-        <f t="shared" si="14"/>
-        <v>6.3702834161542956</v>
+        <f t="shared" si="13"/>
+        <v>8.5616609113113729</v>
       </c>
     </row>
     <row r="19" spans="8:15" x14ac:dyDescent="0.75">
@@ -949,26 +936,26 @@
         <v>0.25</v>
       </c>
       <c r="O19" s="2">
-        <f t="shared" si="14"/>
-        <v>-0.16846370252175669</v>
+        <f t="shared" si="13"/>
+        <v>-0.22641521618924099</v>
       </c>
     </row>
     <row r="21" spans="8:15" x14ac:dyDescent="0.75">
       <c r="N21" t="s">
         <v>12</v>
       </c>
-      <c r="O21" s="8">
+      <c r="O21" s="5">
         <f>SUMPRODUCT(O16:O19,N16:N19)</f>
-        <v>13.209775784773816</v>
+        <v>17.753938654736011</v>
       </c>
     </row>
     <row r="22" spans="8:15" x14ac:dyDescent="0.75">
       <c r="N22" t="s">
         <v>11</v>
       </c>
-      <c r="O22" s="8">
+      <c r="O22" s="5">
         <f t="array" ref="O22">MMULT(TRANSPOSE(N16:N19),O16:O19)</f>
-        <v>13.209775784773816</v>
+        <v>17.753938654736011</v>
       </c>
     </row>
     <row r="24" spans="8:15" x14ac:dyDescent="0.75">
@@ -977,16 +964,16 @@
       </c>
       <c r="O24" cm="1">
         <f t="array" ref="O24">SQRT(MMULT(MMULT(TRANSPOSE($N$16:$N$19),$Q$5:$T$8),$N$16:$N$19))</f>
-        <v>1.6802832634972789</v>
+        <v>1.8998165646586371</v>
       </c>
     </row>
     <row r="25" spans="8:15" x14ac:dyDescent="0.75">
       <c r="N25" t="s">
         <v>14</v>
       </c>
-      <c r="O25" s="9">
+      <c r="O25" s="6">
         <f>O21/O24</f>
-        <v>7.8616362322621018</v>
+        <v>9.3450804593474395</v>
       </c>
     </row>
     <row r="27" spans="8:15" x14ac:dyDescent="0.75">
@@ -995,39 +982,39 @@
       </c>
     </row>
     <row r="28" spans="8:15" x14ac:dyDescent="0.75">
-      <c r="N28" s="10">
+      <c r="N28" s="7">
         <v>0.99991948501333083</v>
       </c>
       <c r="O28" s="2">
         <f>O16</f>
-        <v>0.29145275964966716</v>
+        <v>0.39171250896915266</v>
       </c>
     </row>
     <row r="29" spans="8:15" x14ac:dyDescent="0.75">
-      <c r="N29" s="10">
+      <c r="N29" s="7">
         <v>8.0514986668684779E-5</v>
       </c>
       <c r="O29" s="2">
-        <f t="shared" ref="O29:O31" si="16">O17</f>
-        <v>46.345830665813061</v>
+        <f t="shared" ref="O29:O31" si="15">O17</f>
+        <v>62.288796414852754</v>
       </c>
     </row>
     <row r="30" spans="8:15" x14ac:dyDescent="0.75">
-      <c r="N30" s="10">
+      <c r="N30" s="7">
         <v>0</v>
       </c>
       <c r="O30" s="2">
-        <f t="shared" si="16"/>
-        <v>6.3702834161542956</v>
+        <f t="shared" si="15"/>
+        <v>8.5616609113113729</v>
       </c>
     </row>
     <row r="31" spans="8:15" x14ac:dyDescent="0.75">
-      <c r="N31" s="10">
+      <c r="N31" s="7">
         <v>0</v>
       </c>
       <c r="O31" s="2">
-        <f t="shared" si="16"/>
-        <v>-0.16846370252175669</v>
+        <f t="shared" si="15"/>
+        <v>-0.22641521618924099</v>
       </c>
     </row>
     <row r="32" spans="8:15" x14ac:dyDescent="0.75">
@@ -1035,24 +1022,24 @@
         <f>SUM(N28:N31)</f>
         <v>0.99999999999999956</v>
       </c>
-      <c r="O32" s="8"/>
+      <c r="O32" s="5"/>
     </row>
     <row r="33" spans="14:15" x14ac:dyDescent="0.75">
       <c r="N33" t="s">
         <v>15</v>
       </c>
-      <c r="O33" s="8">
+      <c r="O33" s="5">
         <f>SUMPRODUCT(O28:O31,N28:N31)</f>
-        <v>0.29516082727281634</v>
+        <v>0.39669615185466517</v>
       </c>
     </row>
     <row r="34" spans="14:15" x14ac:dyDescent="0.75">
       <c r="N34" t="s">
         <v>16</v>
       </c>
-      <c r="O34" s="8" cm="1">
+      <c r="O34" s="5" cm="1">
         <f t="array" ref="O34">MMULT(TRANSPOSE(N28:N31),O28:O31)</f>
-        <v>0.29516082727281634</v>
+        <v>0.39669615185466517</v>
       </c>
     </row>
     <row r="36" spans="14:15" x14ac:dyDescent="0.75">
@@ -1061,7 +1048,7 @@
       </c>
       <c r="O36" s="2" cm="1">
         <f t="array" ref="O36">SQRT(MMULT(MMULT(TRANSPOSE($N$28:$N$31),$Q$5:$T$8),$N$28:$N$31))</f>
-        <v>0.14344394774268571</v>
+        <v>1.0466386489798852E-2</v>
       </c>
     </row>
     <row r="38" spans="14:15" x14ac:dyDescent="0.75">
@@ -1070,7 +1057,7 @@
       </c>
       <c r="O38">
         <f>O34/O36</f>
-        <v>2.0576736203766868</v>
+        <v>37.90192080536184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>